<commit_message>
Added payload images of flight
</commit_message>
<xml_diff>
--- a/version06/201503141438.xlsx
+++ b/version06/201503141438.xlsx
@@ -804,8 +804,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289488480"/>
-        <c:axId val="151214392"/>
+        <c:axId val="171765344"/>
+        <c:axId val="171770336"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1464,11 +1464,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149415344"/>
-        <c:axId val="289489264"/>
+        <c:axId val="171775200"/>
+        <c:axId val="171774816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289488480"/>
+        <c:axId val="171765344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,12 +1525,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151214392"/>
+        <c:crossAx val="171770336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151214392"/>
+        <c:axId val="171770336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1587,12 +1587,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289488480"/>
+        <c:crossAx val="171765344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289489264"/>
+        <c:axId val="171774816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,12 +1635,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149415344"/>
+        <c:crossAx val="171775200"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149415344"/>
+        <c:axId val="171775200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1650,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289489264"/>
+        <c:crossAx val="171774816"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2291,14 +2292,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>38099</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2586,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>